<commit_message>
Add new test, fix test data
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/timeline_duration.xlsx
+++ b/tests/integration_test_files/timeline_duration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40084D1B-9FCD-C24B-BF75-15672F4C1595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8117C872-33C5-984D-9706-613316ED4A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="27240" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="4780" yWindow="500" windowWidth="35500" windowHeight="27240" firstSheet="5" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="868">
   <si>
     <t>Screening</t>
   </si>
@@ -2672,6 +2672,24 @@
   </si>
   <si>
     <t>Amendment Four</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>durationDescription</t>
+  </si>
+  <si>
+    <t>reasonDurationWillVary</t>
+  </si>
+  <si>
+    <t>100 Days</t>
+  </si>
+  <si>
+    <t>Because shit happens</t>
+  </si>
+  <si>
+    <t>The length of the study</t>
   </si>
 </sst>
 </file>
@@ -3477,16 +3495,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
     <col min="4" max="8" width="12.33203125" style="1" customWidth="1"/>
@@ -3572,7 +3590,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
+      <c r="A4" s="13" t="s">
+        <v>862</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>865</v>
+      </c>
       <c r="C4" s="13" t="s">
         <v>40</v>
       </c>
@@ -3593,7 +3616,12 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
+      <c r="A5" s="13" t="s">
+        <v>864</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>866</v>
+      </c>
       <c r="C5" s="13" t="s">
         <v>614</v>
       </c>
@@ -3614,7 +3642,12 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
+      <c r="A6" s="13" t="s">
+        <v>863</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>867</v>
+      </c>
       <c r="C6" s="13" t="s">
         <v>616</v>
       </c>
@@ -5304,7 +5337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051C019D-8DBE-D14B-A9B5-0060B58D7557}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>